<commit_message>
Newer version of data file as found & sent by Ellie.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Distraction_Assignment_TG.xlsx
+++ b/raw-data-prep/raw_data/Distraction_Assignment_TG.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
@@ -11,24 +11,36 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Subject</t>
   </si>
   <si>
     <t>Assignment</t>
   </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>square by number</t>
+  </si>
+  <si>
+    <t>triangle by number</t>
+  </si>
+  <si>
+    <t>circle by number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +160,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -182,6 +195,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,35 +371,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>203</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>224</v>
       </c>
@@ -393,15 +413,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>225</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>229</v>
       </c>
@@ -409,7 +432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>230</v>
       </c>
@@ -417,7 +440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>232</v>
       </c>
@@ -425,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>231</v>
       </c>
@@ -433,7 +456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>233</v>
       </c>
@@ -441,7 +464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>234</v>
       </c>
@@ -449,7 +472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>235</v>
       </c>
@@ -457,7 +480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>236</v>
       </c>
@@ -465,7 +488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>237</v>
       </c>
@@ -473,23 +496,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>238</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>239</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>240</v>
       </c>
@@ -497,7 +526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>241</v>
       </c>
@@ -505,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>242</v>
       </c>
@@ -513,7 +542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>243</v>
       </c>
@@ -521,15 +550,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>244</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>245</v>
       </c>
@@ -537,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>246</v>
       </c>
@@ -545,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>247</v>
       </c>
@@ -553,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>248</v>
       </c>
@@ -561,15 +593,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>249</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>250</v>
       </c>
@@ -577,7 +612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>251</v>
       </c>
@@ -585,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>252</v>
       </c>
@@ -593,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>253</v>
       </c>
@@ -601,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>254</v>
       </c>
@@ -609,7 +644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>255</v>
       </c>
@@ -617,15 +652,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>256</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>257</v>
       </c>
@@ -633,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>258</v>
       </c>
@@ -641,15 +679,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>259</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>260</v>
       </c>
@@ -657,15 +698,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>261</v>
       </c>
       <c r="B37">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>262</v>
       </c>
@@ -673,7 +717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>263</v>
       </c>
@@ -681,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>264</v>
       </c>
@@ -689,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>265</v>
       </c>
@@ -697,23 +741,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>266</v>
       </c>
       <c r="B42">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>267</v>
       </c>
       <c r="B43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>268</v>
       </c>
@@ -721,7 +771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>269</v>
       </c>
@@ -729,7 +779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>270</v>
       </c>
@@ -737,7 +787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>271</v>
       </c>
@@ -745,7 +795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>272</v>
       </c>
@@ -753,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>273</v>
       </c>
@@ -761,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>274</v>
       </c>
@@ -769,7 +819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>275</v>
       </c>
@@ -777,15 +827,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>276</v>
       </c>
       <c r="B52">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="D52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>277</v>
       </c>
@@ -793,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>278</v>
       </c>
@@ -801,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>279</v>
       </c>
@@ -809,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>281</v>
       </c>
@@ -817,15 +870,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>282</v>
       </c>
       <c r="B57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>283</v>
       </c>
@@ -833,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>284</v>
       </c>
@@ -841,15 +897,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>285</v>
       </c>
       <c r="B60">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>286</v>
       </c>
@@ -857,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>287</v>
       </c>
@@ -865,7 +924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>290</v>
       </c>
@@ -873,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>291</v>
       </c>
@@ -881,7 +940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>292</v>
       </c>
@@ -889,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>293</v>
       </c>
@@ -897,7 +956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>294</v>
       </c>
@@ -905,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>295</v>
       </c>
@@ -913,7 +972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>296</v>
       </c>
@@ -921,7 +980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>297</v>
       </c>
@@ -929,7 +988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>298</v>
       </c>
@@ -937,15 +996,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>299</v>
       </c>
       <c r="B72">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>300</v>
       </c>
@@ -953,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>301</v>
       </c>
@@ -961,7 +1023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>302</v>
       </c>
@@ -969,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>303</v>
       </c>
@@ -977,7 +1039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>304</v>
       </c>
@@ -985,7 +1047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>305</v>
       </c>
@@ -993,7 +1055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>306</v>
       </c>
@@ -1001,7 +1063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>307</v>
       </c>
@@ -1009,11 +1071,587 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>308</v>
       </c>
       <c r="B81">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>309</v>
+      </c>
+      <c r="B82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>310</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>311</v>
+      </c>
+      <c r="B84">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>312</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>313</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>314</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>316</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>317</v>
+      </c>
+      <c r="B89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>318</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>319</v>
+      </c>
+      <c r="B91">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>320</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>321</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>322</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>323</v>
+      </c>
+      <c r="B95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>324</v>
+      </c>
+      <c r="B96">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>325</v>
+      </c>
+      <c r="B97">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>326</v>
+      </c>
+      <c r="B98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>327</v>
+      </c>
+      <c r="B99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>328</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>329</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>330</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>331</v>
+      </c>
+      <c r="B103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>332</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>333</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>334</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>335</v>
+      </c>
+      <c r="B107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>336</v>
+      </c>
+      <c r="B108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>337</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>338</v>
+      </c>
+      <c r="B110">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>339</v>
+      </c>
+      <c r="B111">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>340</v>
+      </c>
+      <c r="B112">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>341</v>
+      </c>
+      <c r="B113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>342</v>
+      </c>
+      <c r="B114">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>343</v>
+      </c>
+      <c r="B115">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>344</v>
+      </c>
+      <c r="B116">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>345</v>
+      </c>
+      <c r="B117">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>346</v>
+      </c>
+      <c r="B118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>347</v>
+      </c>
+      <c r="B119">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>348</v>
+      </c>
+      <c r="B120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>349</v>
+      </c>
+      <c r="B121">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>350</v>
+      </c>
+      <c r="B122">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>351</v>
+      </c>
+      <c r="B123">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>352</v>
+      </c>
+      <c r="B124">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>353</v>
+      </c>
+      <c r="B125">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>354</v>
+      </c>
+      <c r="B126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>355</v>
+      </c>
+      <c r="B127">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>356</v>
+      </c>
+      <c r="B128">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>357</v>
+      </c>
+      <c r="B129">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>358</v>
+      </c>
+      <c r="B130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>359</v>
+      </c>
+      <c r="B131">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>360</v>
+      </c>
+      <c r="B132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>361</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>362</v>
+      </c>
+      <c r="B134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>363</v>
+      </c>
+      <c r="B135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>364</v>
+      </c>
+      <c r="B136">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>365</v>
+      </c>
+      <c r="B137">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>366</v>
+      </c>
+      <c r="B138">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>367</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>368</v>
+      </c>
+      <c r="B140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>369</v>
+      </c>
+      <c r="B141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>370</v>
+      </c>
+      <c r="B142">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>371</v>
+      </c>
+      <c r="B143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>372</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>373</v>
+      </c>
+      <c r="B145">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>374</v>
+      </c>
+      <c r="B146">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>375</v>
+      </c>
+      <c r="B147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>376</v>
+      </c>
+      <c r="B148">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>377</v>
+      </c>
+      <c r="B149">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>378</v>
+      </c>
+      <c r="B150">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>379</v>
+      </c>
+      <c r="B151">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>380</v>
+      </c>
+      <c r="B152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>381</v>
+      </c>
+      <c r="B153">
         <v>9</v>
       </c>
     </row>
@@ -1023,24 +1661,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed unnecessary columns from Distraction_Assignment_TG.xlsx
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Distraction_Assignment_TG.xlsx
+++ b/raw-data-prep/raw_data/Distraction_Assignment_TG.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard\Documents\GitHub\vg-dissertation\raw-data-prep\raw_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,24 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Subject</t>
   </si>
   <si>
     <t>Assignment</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>square by number</t>
-  </si>
-  <si>
-    <t>triangle by number</t>
-  </si>
-  <si>
-    <t>circle by number</t>
   </si>
 </sst>
 </file>
@@ -80,6 +73,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -128,7 +124,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -163,7 +159,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,29 +379,23 @@
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>203</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>224</v>
       </c>
@@ -413,18 +403,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>225</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>229</v>
       </c>
@@ -432,7 +419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>230</v>
       </c>
@@ -440,7 +427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>232</v>
       </c>
@@ -448,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>231</v>
       </c>
@@ -456,7 +443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>233</v>
       </c>
@@ -464,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>234</v>
       </c>
@@ -472,7 +459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>235</v>
       </c>
@@ -480,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>236</v>
       </c>
@@ -488,7 +475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>237</v>
       </c>
@@ -496,29 +483,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>238</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>239</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>240</v>
       </c>
@@ -526,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>241</v>
       </c>
@@ -534,7 +515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>242</v>
       </c>
@@ -542,7 +523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>243</v>
       </c>
@@ -550,18 +531,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>244</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>245</v>
       </c>
@@ -569,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>246</v>
       </c>
@@ -577,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>247</v>
       </c>
@@ -585,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>248</v>
       </c>
@@ -593,18 +571,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>249</v>
       </c>
       <c r="B25">
         <v>9</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>250</v>
       </c>
@@ -612,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>251</v>
       </c>
@@ -620,7 +595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>252</v>
       </c>
@@ -628,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>253</v>
       </c>
@@ -636,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>254</v>
       </c>
@@ -644,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>255</v>
       </c>
@@ -652,18 +627,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>256</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>257</v>
       </c>
@@ -671,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>258</v>
       </c>
@@ -679,18 +651,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>259</v>
       </c>
       <c r="B35">
         <v>7</v>
       </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>260</v>
       </c>
@@ -698,18 +667,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>261</v>
       </c>
       <c r="B37">
         <v>7</v>
       </c>
-      <c r="D37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>262</v>
       </c>
@@ -717,7 +683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>263</v>
       </c>
@@ -725,7 +691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>264</v>
       </c>
@@ -733,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>265</v>
       </c>
@@ -741,29 +707,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>266</v>
       </c>
       <c r="B42">
         <v>9</v>
       </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>267</v>
       </c>
       <c r="B43">
         <v>5</v>
       </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>268</v>
       </c>
@@ -771,7 +731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>269</v>
       </c>
@@ -779,7 +739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>270</v>
       </c>
@@ -787,7 +747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>271</v>
       </c>
@@ -795,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>272</v>
       </c>
@@ -803,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>273</v>
       </c>
@@ -811,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>274</v>
       </c>
@@ -819,7 +779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>275</v>
       </c>
@@ -827,18 +787,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>276</v>
       </c>
       <c r="B52">
         <v>8</v>
       </c>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>277</v>
       </c>
@@ -846,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>278</v>
       </c>
@@ -854,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>279</v>
       </c>
@@ -862,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>281</v>
       </c>
@@ -870,18 +827,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>282</v>
       </c>
       <c r="B57">
         <v>9</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>283</v>
       </c>
@@ -889,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>284</v>
       </c>
@@ -897,18 +851,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>285</v>
       </c>
       <c r="B60">
         <v>8</v>
       </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>286</v>
       </c>
@@ -916,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>287</v>
       </c>
@@ -924,7 +875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>290</v>
       </c>
@@ -932,7 +883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>291</v>
       </c>
@@ -940,7 +891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>292</v>
       </c>
@@ -948,7 +899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>293</v>
       </c>
@@ -956,7 +907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>294</v>
       </c>
@@ -964,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>295</v>
       </c>
@@ -972,7 +923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>296</v>
       </c>
@@ -980,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>297</v>
       </c>
@@ -988,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>298</v>
       </c>
@@ -996,18 +947,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>299</v>
       </c>
       <c r="B72">
         <v>7</v>
       </c>
-      <c r="C72">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>300</v>
       </c>
@@ -1015,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>301</v>
       </c>
@@ -1023,7 +971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>302</v>
       </c>
@@ -1031,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>303</v>
       </c>
@@ -1039,7 +987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>304</v>
       </c>
@@ -1047,7 +995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>305</v>
       </c>
@@ -1055,7 +1003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>306</v>
       </c>
@@ -1063,7 +1011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>307</v>
       </c>

</xml_diff>